<commit_message>
Finalizando o PPT - 13/03/2024 - Leo
</commit_message>
<xml_diff>
--- a/aaa.xlsx
+++ b/aaa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leova\Desktop\Projetos\05_modelo_risco_de_credito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA9BECD4-910D-498C-89B2-E0FB540EFA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605020A4-3674-423D-B809-DD8ED970CC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="19200" windowWidth="16200" windowHeight="19200" xr2:uid="{23B778D9-052D-4635-9104-521E239C5A58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{23B778D9-052D-4635-9104-521E239C5A58}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -821,7 +821,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>